<commit_message>
Updating BCIO intervention development.xlsx
</commit_message>
<xml_diff>
--- a/Intervention development/BCIO intervention development.xlsx
+++ b/Intervention development/BCIO intervention development.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,26 +560,30 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr"/>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050273</t>
+        </is>
+      </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">behaviour change intervention development process </t>
+          <t>agent</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr"/>
-      <c r="D2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>An independent continuant that is a human being, group or organisation.</t>
+        </is>
+      </c>
       <c r="E2" s="2" t="inlineStr"/>
       <c r="F2" s="2" t="inlineStr"/>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>intervention development process</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
+          <t>independent continuant</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="inlineStr">
         <is>
           <t>Intervention development</t>
@@ -595,9 +599,7 @@
       <c r="Q2" s="2" t="inlineStr"/>
       <c r="R2" s="2" t="inlineStr"/>
       <c r="S2" s="2" t="inlineStr"/>
-      <c r="T2" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="T2" s="2" t="inlineStr"/>
       <c r="U2" s="2" t="inlineStr"/>
       <c r="V2" s="2" t="inlineStr">
         <is>
@@ -613,27 +615,19 @@
       <c r="Y2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>BCIO:050269</t>
-        </is>
-      </c>
+      <c r="A3" s="2" t="inlineStr"/>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>co-production</t>
+          <t xml:space="preserve">behaviour change intervention development process </t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr"/>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>A development process in which the instigators of the development involve other stakeholders as development partners.</t>
-        </is>
-      </c>
+      <c r="D3" s="2" t="inlineStr"/>
       <c r="E3" s="2" t="inlineStr"/>
       <c r="F3" s="2" t="inlineStr"/>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>development process</t>
+          <t>intervention development process</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -656,11 +650,17 @@
       <c r="Q3" s="2" t="inlineStr"/>
       <c r="R3" s="2" t="inlineStr"/>
       <c r="S3" s="2" t="inlineStr"/>
-      <c r="T3" s="2" t="n">
-        <v>0</v>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U3" s="2" t="inlineStr"/>
-      <c r="V3" s="2" t="inlineStr"/>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
       <c r="W3" s="2" t="inlineStr">
         <is>
           <t>Proposed</t>
@@ -672,18 +672,18 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>BCIO:050270</t>
+          <t>BCIO:050269</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>collaboration process</t>
+          <t>co-production</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr"/>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>A process</t>
+          <t>A development process in which developers involve other stakeholders as development partners.</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr"/>
@@ -713,8 +713,10 @@
       <c r="Q4" s="2" t="inlineStr"/>
       <c r="R4" s="2" t="inlineStr"/>
       <c r="S4" s="2" t="inlineStr"/>
-      <c r="T4" s="2" t="n">
-        <v>0</v>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U4" s="2" t="inlineStr"/>
       <c r="V4" s="2" t="inlineStr">
@@ -731,14 +733,22 @@
       <c r="Y4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr"/>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050270</t>
+        </is>
+      </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>consultation2</t>
+          <t>collaboration process</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr"/>
-      <c r="D5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>A process</t>
+        </is>
+      </c>
       <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="inlineStr"/>
       <c r="G5" s="2" t="inlineStr">
@@ -766,8 +776,10 @@
       <c r="Q5" s="2" t="inlineStr"/>
       <c r="R5" s="2" t="inlineStr"/>
       <c r="S5" s="2" t="inlineStr"/>
-      <c r="T5" s="2" t="n">
-        <v>0</v>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U5" s="2" t="inlineStr"/>
       <c r="V5" s="2" t="inlineStr">
@@ -787,7 +799,7 @@
       <c r="A6" s="2" t="inlineStr"/>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>developer role</t>
+          <t>consultation</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr"/>
@@ -796,7 +808,7 @@
       <c r="F6" s="2" t="inlineStr"/>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>role</t>
+          <t>development process</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
@@ -819,8 +831,10 @@
       <c r="Q6" s="2" t="inlineStr"/>
       <c r="R6" s="2" t="inlineStr"/>
       <c r="S6" s="2" t="inlineStr"/>
-      <c r="T6" s="2" t="n">
-        <v>0</v>
+      <c r="T6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U6" s="2" t="inlineStr"/>
       <c r="V6" s="2" t="inlineStr">
@@ -837,55 +851,65 @@
       <c r="Y6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>development partner</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>A person, group or organisation that has a development partner role.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>('human being' or 'group' or 'organisation') and ('has role' 'development partner role')</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>development partner role</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050274</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>developer</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr"/>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>An agent with a developer role.</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>Intervention development</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr"/>
+      <c r="K7" s="2" t="inlineStr"/>
+      <c r="L7" s="2" t="inlineStr"/>
+      <c r="M7" s="2" t="inlineStr"/>
+      <c r="N7" s="2" t="inlineStr"/>
+      <c r="O7" s="2" t="inlineStr"/>
+      <c r="P7" s="2" t="inlineStr"/>
+      <c r="Q7" s="2" t="inlineStr"/>
+      <c r="R7" s="2" t="inlineStr"/>
+      <c r="S7" s="2" t="inlineStr"/>
+      <c r="T7" s="2" t="inlineStr"/>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
+      <c r="W7" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="X7" s="2" t="inlineStr"/>
+      <c r="Y7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>development partner role</t>
+          <t>developer role</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr"/>
@@ -899,7 +923,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>independent continuant</t>
+          <t>process</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
@@ -917,8 +941,10 @@
       <c r="Q8" s="2" t="inlineStr"/>
       <c r="R8" s="2" t="inlineStr"/>
       <c r="S8" s="2" t="inlineStr"/>
-      <c r="T8" s="2" t="n">
-        <v>0</v>
+      <c r="T8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U8" s="2" t="inlineStr"/>
       <c r="V8" s="2" t="inlineStr">
@@ -937,32 +963,32 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>BCIO:050271</t>
+          <t>BCIO:050275</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>development process</t>
+          <t>development partner</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr"/>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>A process that is creation a product, commodity, service or intervention.</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr"/>
+          <t>A person, group or organisation that has a development partner role.</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>('human being' or 'group' or 'organisation') and ('has role' 'development partner role')</t>
+        </is>
+      </c>
       <c r="F9" s="2" t="inlineStr"/>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>planned process</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr"/>
       <c r="I9" s="2" t="inlineStr">
         <is>
           <t>Intervention development</t>
@@ -971,15 +997,21 @@
       <c r="J9" s="2" t="inlineStr"/>
       <c r="K9" s="2" t="inlineStr"/>
       <c r="L9" s="2" t="inlineStr"/>
-      <c r="M9" s="2" t="inlineStr"/>
+      <c r="M9" s="2" t="inlineStr">
+        <is>
+          <t>development partner role</t>
+        </is>
+      </c>
       <c r="N9" s="2" t="inlineStr"/>
       <c r="O9" s="2" t="inlineStr"/>
       <c r="P9" s="2" t="inlineStr"/>
       <c r="Q9" s="2" t="inlineStr"/>
       <c r="R9" s="2" t="inlineStr"/>
       <c r="S9" s="2" t="inlineStr"/>
-      <c r="T9" s="2" t="n">
-        <v>0</v>
+      <c r="T9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U9" s="2" t="inlineStr"/>
       <c r="V9" s="2" t="inlineStr">
@@ -999,7 +1031,7 @@
       <c r="A10" s="2" t="inlineStr"/>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>engagement</t>
+          <t>development partner role</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr"/>
@@ -1008,12 +1040,12 @@
       <c r="F10" s="2" t="inlineStr"/>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>development process</t>
+          <t>role</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>process</t>
+          <t>independent continuant</t>
         </is>
       </c>
       <c r="I10" s="2" t="inlineStr">
@@ -1031,8 +1063,10 @@
       <c r="Q10" s="2" t="inlineStr"/>
       <c r="R10" s="2" t="inlineStr"/>
       <c r="S10" s="2" t="inlineStr"/>
-      <c r="T10" s="2" t="n">
-        <v>0</v>
+      <c r="T10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U10" s="2" t="inlineStr"/>
       <c r="V10" s="2" t="inlineStr">
@@ -1049,19 +1083,27 @@
       <c r="Y10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr"/>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050271</t>
+        </is>
+      </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>intervention development process</t>
+          <t>development process</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr"/>
-      <c r="D11" s="2" t="inlineStr"/>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>A process that is creation a product, commodity, service or intervention.</t>
+        </is>
+      </c>
       <c r="E11" s="2" t="inlineStr"/>
       <c r="F11" s="2" t="inlineStr"/>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>development process</t>
+          <t>planned process</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr">
@@ -1084,8 +1126,10 @@
       <c r="Q11" s="2" t="inlineStr"/>
       <c r="R11" s="2" t="inlineStr"/>
       <c r="S11" s="2" t="inlineStr"/>
-      <c r="T11" s="2" t="n">
-        <v>0</v>
+      <c r="T11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U11" s="2" t="inlineStr"/>
       <c r="V11" s="2" t="inlineStr">
@@ -1105,7 +1149,7 @@
       <c r="A12" s="2" t="inlineStr"/>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>patient and public involvement</t>
+          <t>engagement</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
@@ -1137,8 +1181,10 @@
       <c r="Q12" s="2" t="inlineStr"/>
       <c r="R12" s="2" t="inlineStr"/>
       <c r="S12" s="2" t="inlineStr"/>
-      <c r="T12" s="2" t="n">
-        <v>0</v>
+      <c r="T12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U12" s="2" t="inlineStr"/>
       <c r="V12" s="2" t="inlineStr">
@@ -1158,7 +1204,7 @@
       <c r="A13" s="2" t="inlineStr"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>patient and public involvement and engagement</t>
+          <t>intervention development process</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
@@ -1190,8 +1236,10 @@
       <c r="Q13" s="2" t="inlineStr"/>
       <c r="R13" s="2" t="inlineStr"/>
       <c r="S13" s="2" t="inlineStr"/>
-      <c r="T13" s="2" t="n">
-        <v>0</v>
+      <c r="T13" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U13" s="2" t="inlineStr"/>
       <c r="V13" s="2" t="inlineStr">
@@ -1211,7 +1259,7 @@
       <c r="A14" s="2" t="inlineStr"/>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>product development process</t>
+          <t>patient and public involvement</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr"/>
@@ -1243,8 +1291,10 @@
       <c r="Q14" s="2" t="inlineStr"/>
       <c r="R14" s="2" t="inlineStr"/>
       <c r="S14" s="2" t="inlineStr"/>
-      <c r="T14" s="2" t="n">
-        <v>0</v>
+      <c r="T14" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U14" s="2" t="inlineStr"/>
       <c r="V14" s="2" t="inlineStr">
@@ -1264,7 +1314,7 @@
       <c r="A15" s="2" t="inlineStr"/>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>project development process</t>
+          <t>patient and public involvement and engagement</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr"/>
@@ -1296,8 +1346,10 @@
       <c r="Q15" s="2" t="inlineStr"/>
       <c r="R15" s="2" t="inlineStr"/>
       <c r="S15" s="2" t="inlineStr"/>
-      <c r="T15" s="2" t="n">
-        <v>0</v>
+      <c r="T15" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U15" s="2" t="inlineStr"/>
       <c r="V15" s="2" t="inlineStr">
@@ -1317,7 +1369,7 @@
       <c r="A16" s="2" t="inlineStr"/>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>service development process</t>
+          <t>product development process</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr"/>
@@ -1349,8 +1401,10 @@
       <c r="Q16" s="2" t="inlineStr"/>
       <c r="R16" s="2" t="inlineStr"/>
       <c r="S16" s="2" t="inlineStr"/>
-      <c r="T16" s="2" t="n">
-        <v>0</v>
+      <c r="T16" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U16" s="2" t="inlineStr"/>
       <c r="V16" s="2" t="inlineStr">
@@ -1367,73 +1421,79 @@
       <c r="Y16" s="2" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>stakeholder</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>A person, group or organisation that has a stakeholder role.</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>stakeholder role</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="n">
-        <v>0</v>
-      </c>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
+      <c r="A17" s="2" t="inlineStr"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>project development process</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr"/>
+      <c r="D17" s="2" t="inlineStr"/>
+      <c r="E17" s="2" t="inlineStr"/>
+      <c r="F17" s="2" t="inlineStr"/>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>development process</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="I17" s="2" t="inlineStr">
+        <is>
+          <t>Intervention development</t>
+        </is>
+      </c>
+      <c r="J17" s="2" t="inlineStr"/>
+      <c r="K17" s="2" t="inlineStr"/>
+      <c r="L17" s="2" t="inlineStr"/>
+      <c r="M17" s="2" t="inlineStr"/>
+      <c r="N17" s="2" t="inlineStr"/>
+      <c r="O17" s="2" t="inlineStr"/>
+      <c r="P17" s="2" t="inlineStr"/>
+      <c r="Q17" s="2" t="inlineStr"/>
+      <c r="R17" s="2" t="inlineStr"/>
+      <c r="S17" s="2" t="inlineStr"/>
+      <c r="T17" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U17" s="2" t="inlineStr"/>
+      <c r="V17" s="2" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
+      <c r="W17" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="X17" s="2" t="inlineStr"/>
+      <c r="Y17" s="2" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>BCIO:050272</t>
-        </is>
-      </c>
+      <c r="A18" s="2" t="inlineStr"/>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>stakeholder role</t>
+          <t>service development process</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr"/>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>A role that is being involved with or affected by a project, service, intervention, commodity, product or enterprise.</t>
-        </is>
-      </c>
+      <c r="D18" s="2" t="inlineStr"/>
       <c r="E18" s="2" t="inlineStr"/>
       <c r="F18" s="2" t="inlineStr"/>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>role</t>
+          <t>development process</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>independent continuant</t>
+          <t>process</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr">
@@ -1451,8 +1511,10 @@
       <c r="Q18" s="2" t="inlineStr"/>
       <c r="R18" s="2" t="inlineStr"/>
       <c r="S18" s="2" t="inlineStr"/>
-      <c r="T18" s="2" t="n">
-        <v>0</v>
+      <c r="T18" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="U18" s="2" t="inlineStr"/>
       <c r="V18" s="2" t="inlineStr">
@@ -1467,6 +1529,132 @@
       </c>
       <c r="X18" s="2" t="inlineStr"/>
       <c r="Y18" s="2" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050276</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>stakeholder</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr"/>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>A person, group or organisation that has a stakeholder role.</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr"/>
+      <c r="F19" s="2" t="inlineStr"/>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="inlineStr"/>
+      <c r="I19" s="2" t="inlineStr">
+        <is>
+          <t>Intervention development</t>
+        </is>
+      </c>
+      <c r="J19" s="2" t="inlineStr"/>
+      <c r="K19" s="2" t="inlineStr"/>
+      <c r="L19" s="2" t="inlineStr"/>
+      <c r="M19" s="2" t="inlineStr">
+        <is>
+          <t>stakeholder role</t>
+        </is>
+      </c>
+      <c r="N19" s="2" t="inlineStr"/>
+      <c r="O19" s="2" t="inlineStr"/>
+      <c r="P19" s="2" t="inlineStr"/>
+      <c r="Q19" s="2" t="inlineStr"/>
+      <c r="R19" s="2" t="inlineStr"/>
+      <c r="S19" s="2" t="inlineStr"/>
+      <c r="T19" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U19" s="2" t="inlineStr"/>
+      <c r="V19" s="2" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
+      <c r="W19" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="X19" s="2" t="inlineStr"/>
+      <c r="Y19" s="2" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050272</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>stakeholder role</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr"/>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>A role that is being involved with or affected by a project, service, intervention, commodity, product or enterprise.</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr"/>
+      <c r="F20" s="2" t="inlineStr"/>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>independent continuant</t>
+        </is>
+      </c>
+      <c r="I20" s="2" t="inlineStr">
+        <is>
+          <t>Intervention development</t>
+        </is>
+      </c>
+      <c r="J20" s="2" t="inlineStr"/>
+      <c r="K20" s="2" t="inlineStr"/>
+      <c r="L20" s="2" t="inlineStr"/>
+      <c r="M20" s="2" t="inlineStr"/>
+      <c r="N20" s="2" t="inlineStr"/>
+      <c r="O20" s="2" t="inlineStr"/>
+      <c r="P20" s="2" t="inlineStr"/>
+      <c r="Q20" s="2" t="inlineStr"/>
+      <c r="R20" s="2" t="inlineStr"/>
+      <c r="S20" s="2" t="inlineStr"/>
+      <c r="T20" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U20" s="2" t="inlineStr"/>
+      <c r="V20" s="2" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
+      <c r="W20" s="2" t="inlineStr">
+        <is>
+          <t>Proposed</t>
+        </is>
+      </c>
+      <c r="X20" s="2" t="inlineStr"/>
+      <c r="Y20" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>